<commit_message>
update layout html exercise
</commit_message>
<xml_diff>
--- a/references/exercises.xlsx
+++ b/references/exercises.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0CCB7E63-F625-4CB5-9488-47172C4446C1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{653777C0-CED5-4E2F-8468-F5CBF8285DA5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
   <si>
     <t>#</t>
   </si>
@@ -108,13 +108,175 @@
   </si>
   <si>
     <t>Trương Công Trường</t>
+  </si>
+  <si>
+    <t>thanhvuongsk/aptech-php-14-vuongnguyen</t>
+  </si>
+  <si>
+    <t>08.04.2018</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>vuanhmai2233/aptech-php-14-vuma</t>
+  </si>
+  <si>
+    <t>manhha2018/aptech-php14-manhha</t>
+  </si>
+  <si>
+    <r>
+      <t>xuanvien890</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF586069"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF0366D6"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>aptech-php-14-xuanvien890</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>nguyenhuan1994dn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF586069"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF0366D6"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>aptech-php-14-nguyenhuan</t>
+    </r>
+  </si>
+  <si>
+    <t>thienpn1/aptech-php-14-hoangthien</t>
+  </si>
+  <si>
+    <r>
+      <t>datnguyen306</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF586069"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF0366D6"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>aptech-php-14-datnb</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>hoanvudn94</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF586069"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF0366D6"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>aptech-php-14-leviethoanvu</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>hongphong93</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF586069"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF0366D6"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>aptech-php-14-phongdvh</t>
+    </r>
+  </si>
+  <si>
+    <t>aptech-php-14-huy-2018-08-04</t>
+  </si>
+  <si>
+    <r>
+      <t>nvphongbk</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF586069"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF0366D6"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>aptech-php-14-nguyenvanphong</t>
+    </r>
+  </si>
+  <si>
+    <t>v</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +296,26 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF586069"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF0366D6"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -143,7 +325,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -196,11 +378,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -209,8 +403,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -574,10 +779,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:C19"/>
+  <dimension ref="A3:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,7 +791,7 @@
     <col min="3" max="3" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -596,80 +801,123 @@
       <c r="C3" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="D3" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C5" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C6" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="81" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C7" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="81" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C8" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C9" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C11" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -677,8 +925,11 @@
         <v>9</v>
       </c>
       <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -686,26 +937,39 @@
         <v>10</v>
       </c>
       <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="81" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C15" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -714,25 +978,30 @@
       </c>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>14</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C17" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C18" s="10"/>
+    </row>
+    <row r="19" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -740,8 +1009,18 @@
         <v>16</v>
       </c>
       <c r="C19" s="2"/>
+      <c r="D19" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C14" r:id="rId1" display="https://github.com/thanhvuongsk/aptech-php-14-vuongnguyen" xr:uid="{E7B9F0F2-3C02-4CB6-AD17-7134235E9DF5}"/>
+    <hyperlink ref="C4" r:id="rId2" display="https://github.com/manhha2018/aptech-php14-manhha" xr:uid="{0086E304-7F94-416E-966E-C431D4B81ED4}"/>
+    <hyperlink ref="C17" r:id="rId3" display="https://github.com/thienpn1/aptech-php-14-hoangthien" xr:uid="{A734A422-70FF-4D6E-9F94-119D716E8B2F}"/>
+    <hyperlink ref="C11" r:id="rId4" display="https://github.com/huyho95/aptech-php-14-huy-2018-08-04" xr:uid="{516B7CC1-8C6A-4ED9-81E9-0D7BECE1B17F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>